<commit_message>
Delete unused file and chenge wording on exele forms.
</commit_message>
<xml_diff>
--- a/Estimation.WebApi/Forms/Estimation_DetailForm.xlsx
+++ b/Estimation.WebApi/Forms/Estimation_DetailForm.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mattanapol.K\Source\Repos\EstimationServer\Estimation.WebApi\Forms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{CF0F278F-F831-4B1E-B88E-5A4F6B712944}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{085578F9-FCBF-4A35-BB4A-83516795340A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -38,9 +38,6 @@
     <t>Date: ##Date##</t>
   </si>
   <si>
-    <t>Code</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -168,6 +165,9 @@
   </si>
   <si>
     <t>Total of ##GROUPCODE##</t>
+  </si>
+  <si>
+    <t>Item</t>
   </si>
 </sst>
 </file>
@@ -235,7 +235,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -299,184 +299,6 @@
     </border>
     <border>
       <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-0.14996795556505021"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.14996795556505021"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.14996795556505021"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-0.14996795556505021"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.14996795556505021"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.14996795556505021"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.14996795556505021"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-0.14996795556505021"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.14996795556505021"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.14996795556505021"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.14996795556505021"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-0.14996795556505021"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.14996795556505021"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.14996795556505021"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.14996795556505021"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.14996795556505021"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.14996795556505021"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.14996795556505021"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-0.14996795556505021"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.14996795556505021"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF808080"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.14996795556505021"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-0.14996795556505021"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-0.14996795556505021"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.14996795556505021"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.14996795556505021"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-0.14996795556505021"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.14996795556505021"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.14996795556505021"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.14996795556505021"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.14993743705557422"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.14996795556505021"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.14993743705557422"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="thin">
@@ -584,53 +406,113 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color theme="0" tint="-0.14996795556505021"/>
+        <color theme="0" tint="-0.34998626667073579"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color theme="0" tint="-0.14996795556505021"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.14996795556505021"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-0.14996795556505021"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color theme="0" tint="-0.14996795556505021"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.14996795556505021"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
       </left>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color theme="0" tint="-0.14996795556505021"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.14996795556505021"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
       </left>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color theme="0" tint="-0.14996795556505021"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
       </top>
       <bottom style="medium">
         <color rgb="FF000000"/>
@@ -639,16 +521,149 @@
     </border>
     <border>
       <left style="thin">
-        <color theme="0" tint="-0.14996795556505021"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-0.14996795556505021"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
       </right>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -673,59 +688,53 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -733,91 +742,97 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -826,7 +841,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -835,22 +850,22 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1169,7 +1184,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
@@ -1197,7 +1212,7 @@
     </row>
     <row r="2" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -1220,160 +1235,160 @@
       <c r="H3" s="3"/>
     </row>
     <row r="4" spans="1:9" s="5" customFormat="1" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="51" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="C4" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="D4" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="E4" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="F4" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="G4" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="H4" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="8" t="s">
+    </row>
+    <row r="5" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="39"/>
+      <c r="B5" s="40" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
-      <c r="B5" s="10" t="s">
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="43"/>
+    </row>
+    <row r="6" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="13"/>
-    </row>
-    <row r="6" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="B6" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="C6" s="33">
+        <v>1</v>
+      </c>
+      <c r="D6" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="16">
+      <c r="E6" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="31" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="32"/>
+      <c r="B7" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="33">
         <v>1</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D7" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="F7" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="G7" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="H7" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
-      <c r="B7" s="15" t="s">
+    </row>
+    <row r="8" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="32"/>
+      <c r="B8" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C8" s="33">
         <v>1</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D8" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="F8" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="G8" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" s="18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
-      <c r="B8" s="16" t="s">
+      <c r="H8" s="31"/>
+    </row>
+    <row r="9" spans="1:9" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="32"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="16">
-        <v>1</v>
-      </c>
-      <c r="D8" s="16" t="s">
+      <c r="D9" s="54"/>
+      <c r="E9" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="17" t="s">
+      <c r="F9" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="17" t="s">
+      <c r="G9" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="H8" s="18"/>
-    </row>
-    <row r="9" spans="1:9" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="14"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="54" t="s">
+      <c r="H9" s="31"/>
+    </row>
+    <row r="10" spans="1:9" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="44"/>
+      <c r="B10" s="45"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="49"/>
+      <c r="H10" s="46"/>
+    </row>
+    <row r="11" spans="1:9" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="6"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="54"/>
-      <c r="E9" s="19" t="s">
+      <c r="D11" s="56"/>
+      <c r="E11" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="19" t="s">
+      <c r="G11" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="H9" s="25"/>
-    </row>
-    <row r="10" spans="1:9" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="23"/>
-      <c r="B10" s="24"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="26"/>
-    </row>
-    <row r="11" spans="1:9" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="27"/>
-      <c r="B11" s="28"/>
-      <c r="C11" s="56" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="56"/>
-      <c r="E11" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="G11" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="H11" s="30"/>
+      <c r="H11" s="9"/>
     </row>
     <row r="12" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
@@ -1393,7 +1408,7 @@
     <mergeCell ref="C11:D11"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.39370078740157483" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="71" fitToWidth="0" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="71" fitToWidth="0" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1401,24 +1416,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63923CB7-A615-4508-8658-19D77FD5F6B4}">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.140625" style="31" customWidth="1"/>
-    <col min="2" max="2" width="32.42578125" style="31" customWidth="1"/>
-    <col min="3" max="4" width="12.7109375" style="31" customWidth="1"/>
-    <col min="5" max="8" width="18.28515625" style="31" customWidth="1"/>
-    <col min="9" max="9" width="22.85546875" style="31" customWidth="1"/>
-    <col min="10" max="10" width="29.42578125" style="31" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="31"/>
+    <col min="1" max="1" width="28.140625" style="10" customWidth="1"/>
+    <col min="2" max="2" width="32.42578125" style="10" customWidth="1"/>
+    <col min="3" max="4" width="12.7109375" style="10" customWidth="1"/>
+    <col min="5" max="8" width="18.28515625" style="10" customWidth="1"/>
+    <col min="9" max="9" width="22.85546875" style="10" customWidth="1"/>
+    <col min="10" max="10" width="29.42578125" style="10" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="59" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B1" s="59"/>
       <c r="C1" s="59"/>
@@ -1431,292 +1446,292 @@
       <c r="J1" s="59"/>
     </row>
     <row r="2" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="33" t="s">
+      <c r="A2" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="12" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="32"/>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-    </row>
-    <row r="4" spans="1:10" s="34" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+    </row>
+    <row r="4" spans="1:10" s="13" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="60" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" s="62" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="62" t="s">
+      <c r="D4" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="62" t="s">
+      <c r="E4" s="62" t="s">
         <v>5</v>
-      </c>
-      <c r="E4" s="62" t="s">
-        <v>6</v>
       </c>
       <c r="F4" s="62"/>
       <c r="G4" s="62" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H4" s="62"/>
       <c r="I4" s="62" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="64" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" s="34" customFormat="1" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:10" s="13" customFormat="1" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="61"/>
       <c r="B5" s="63"/>
       <c r="C5" s="63"/>
       <c r="D5" s="63"/>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" s="35" t="s">
+      <c r="G5" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="14" t="s">
         <v>25</v>
-      </c>
-      <c r="H5" s="35" t="s">
-        <v>26</v>
       </c>
       <c r="I5" s="63"/>
       <c r="J5" s="65"/>
     </row>
     <row r="6" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="36" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="37"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="37"/>
-      <c r="J6" s="38"/>
+      <c r="A6" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="17"/>
     </row>
     <row r="7" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="23"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="26" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="40"/>
-      <c r="C7" s="41"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="41"/>
-      <c r="H7" s="41"/>
-      <c r="I7" s="42"/>
-      <c r="J7" s="43" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="44" t="s">
+      <c r="B8" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="C8" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="D8" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="E8" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="17" t="s">
+      <c r="F8" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="F8" s="17" t="s">
+      <c r="G8" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="G8" s="17" t="s">
+      <c r="H8" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="H8" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="I8" s="17" t="s">
+      <c r="J8" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="J8" s="18" t="s">
+    </row>
+    <row r="9" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="32"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="31"/>
+    </row>
+    <row r="10" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="27" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="18"/>
-    </row>
-    <row r="10" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="44" t="s">
+      <c r="B10" s="28"/>
+      <c r="C10" s="29">
+        <v>1</v>
+      </c>
+      <c r="D10" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="30"/>
+      <c r="F10" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="17">
+      <c r="G10" s="30"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="J10" s="31"/>
+    </row>
+    <row r="11" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="28"/>
+      <c r="C11" s="29">
         <v>1</v>
       </c>
-      <c r="D10" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="16"/>
-      <c r="F10" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="J10" s="18"/>
-    </row>
-    <row r="11" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="44" t="s">
+      <c r="D11" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="30"/>
+      <c r="F11" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="17">
+      <c r="G11" s="30"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="J11" s="31"/>
+    </row>
+    <row r="12" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="28"/>
+      <c r="C12" s="29">
         <v>1</v>
       </c>
-      <c r="D11" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="16"/>
-      <c r="F11" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="J11" s="18"/>
-    </row>
-    <row r="12" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="44" t="s">
+      <c r="D12" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="30"/>
+      <c r="F12" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="17">
+      <c r="G12" s="30"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="J12" s="31"/>
+    </row>
+    <row r="13" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="28"/>
+      <c r="C13" s="29">
         <v>1</v>
       </c>
-      <c r="D12" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" s="16"/>
-      <c r="F12" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="J12" s="18"/>
-    </row>
-    <row r="13" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="44" t="s">
+      <c r="D13" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="30"/>
+      <c r="F13" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="17">
-        <v>1</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" s="16"/>
-      <c r="F13" s="17" t="s">
+      <c r="G13" s="30"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="J13" s="31"/>
+    </row>
+    <row r="14" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="27"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="57" t="s">
         <v>44</v>
-      </c>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="J13" s="18"/>
-    </row>
-    <row r="14" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="44"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="57" t="s">
-        <v>45</v>
       </c>
       <c r="D14" s="57"/>
       <c r="E14" s="57"/>
-      <c r="F14" s="17" t="s">
+      <c r="F14" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17" t="s">
+      <c r="I14" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="I14" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="J14" s="18"/>
+      <c r="J14" s="31"/>
     </row>
     <row r="15" spans="1:10" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="45"/>
-      <c r="B15" s="46"/>
-      <c r="C15" s="47"/>
-      <c r="D15" s="47"/>
-      <c r="E15" s="48"/>
-      <c r="F15" s="48"/>
-      <c r="G15" s="48"/>
-      <c r="H15" s="48"/>
-      <c r="I15" s="48"/>
-      <c r="J15" s="49"/>
+      <c r="A15" s="34"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="37"/>
+      <c r="I15" s="37"/>
+      <c r="J15" s="38"/>
     </row>
     <row r="16" spans="1:10" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="50"/>
-      <c r="B16" s="51"/>
+      <c r="A16" s="18"/>
+      <c r="B16" s="19"/>
       <c r="C16" s="58" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D16" s="58"/>
       <c r="E16" s="58"/>
       <c r="F16" s="58"/>
       <c r="G16" s="58"/>
-      <c r="H16" s="52" t="s">
-        <v>16</v>
-      </c>
-      <c r="I16" s="52" t="s">
-        <v>16</v>
-      </c>
-      <c r="J16" s="53"/>
+      <c r="H16" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="I16" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="J16" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -1733,6 +1748,6 @@
     <mergeCell ref="J4:J5"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.39370078740157483" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="60" fitToWidth="0" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="60" fitToWidth="0" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update form from customer request.
</commit_message>
<xml_diff>
--- a/Estimation.WebApi/Forms/Estimation_DetailForm.xlsx
+++ b/Estimation.WebApi/Forms/Estimation_DetailForm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mattanapol.K\Source\Repos\EstimationServer\Estimation.WebApi\Forms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{085578F9-FCBF-4A35-BB4A-83516795340A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FA186AB-2BFA-4A22-BA7E-D1930B48931C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="43">
   <si>
     <t>SUMMARY OF ESTIMATE</t>
   </si>
@@ -101,24 +101,12 @@
     <t>DESCRIPTION OF ESTIMATE</t>
   </si>
   <si>
-    <t>Material</t>
-  </si>
-  <si>
     <t>Unit Price</t>
   </si>
   <si>
     <t>Amount</t>
   </si>
   <si>
-    <t>##GROUPCODE##) ##GROUPNAME##</t>
-  </si>
-  <si>
-    <t>##NAME##</t>
-  </si>
-  <si>
-    <t>##DESCRIPTION##</t>
-  </si>
-  <si>
     <t>##QUANTITY##</t>
   </si>
   <si>
@@ -168,6 +156,9 @@
   </si>
   <si>
     <t>Item</t>
+  </si>
+  <si>
+    <t>##NAME## - ##DESCRIPTION##</t>
   </si>
 </sst>
 </file>
@@ -671,7 +662,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -736,9 +727,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -778,12 +766,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -841,9 +823,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -867,6 +846,15 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1199,16 +1187,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
     </row>
     <row r="2" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -1235,150 +1223,150 @@
       <c r="H3" s="3"/>
     </row>
     <row r="4" spans="1:9" s="5" customFormat="1" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="51" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4" s="52" t="s">
+      <c r="A4" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="52" t="s">
+      <c r="C4" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="52" t="s">
+      <c r="D4" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="52" t="s">
+      <c r="E4" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="52" t="s">
+      <c r="F4" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="52" t="s">
+      <c r="G4" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="53" t="s">
+      <c r="H4" s="50" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="39"/>
-      <c r="B5" s="40" t="s">
+      <c r="A5" s="36"/>
+      <c r="B5" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="43"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="40"/>
     </row>
     <row r="6" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="33">
+      <c r="C6" s="32">
         <v>1</v>
       </c>
-      <c r="D6" s="33" t="s">
+      <c r="D6" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="29" t="s">
+      <c r="E6" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="29" t="s">
+      <c r="F6" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="29" t="s">
+      <c r="G6" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="31" t="s">
+      <c r="H6" s="30" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="32"/>
-      <c r="B7" s="28" t="s">
+      <c r="A7" s="31"/>
+      <c r="B7" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="33">
+      <c r="C7" s="32">
         <v>1</v>
       </c>
-      <c r="D7" s="33" t="s">
+      <c r="D7" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="29" t="s">
+      <c r="E7" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="29" t="s">
+      <c r="F7" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="29" t="s">
+      <c r="G7" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="31" t="s">
+      <c r="H7" s="30" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="32"/>
-      <c r="B8" s="33" t="s">
+      <c r="A8" s="31"/>
+      <c r="B8" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="33">
+      <c r="C8" s="32">
         <v>1</v>
       </c>
-      <c r="D8" s="33" t="s">
+      <c r="D8" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="29" t="s">
+      <c r="E8" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="29" t="s">
+      <c r="F8" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="29" t="s">
+      <c r="G8" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="31"/>
+      <c r="H8" s="30"/>
     </row>
     <row r="9" spans="1:9" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="32"/>
-      <c r="B9" s="29"/>
-      <c r="C9" s="54" t="s">
+      <c r="A9" s="31"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="54"/>
-      <c r="E9" s="50" t="s">
+      <c r="D9" s="51"/>
+      <c r="E9" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="50" t="s">
+      <c r="F9" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="50" t="s">
+      <c r="G9" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="H9" s="31"/>
+      <c r="H9" s="30"/>
     </row>
     <row r="10" spans="1:9" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="44"/>
-      <c r="B10" s="45"/>
-      <c r="C10" s="47"/>
-      <c r="D10" s="47"/>
-      <c r="E10" s="48"/>
-      <c r="F10" s="48"/>
-      <c r="G10" s="49"/>
-      <c r="H10" s="46"/>
+      <c r="A10" s="41"/>
+      <c r="B10" s="42"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="45"/>
+      <c r="G10" s="46"/>
+      <c r="H10" s="43"/>
     </row>
     <row r="11" spans="1:9" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6"/>
       <c r="B11" s="7"/>
-      <c r="C11" s="56" t="s">
+      <c r="C11" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="56"/>
+      <c r="D11" s="53"/>
       <c r="E11" s="8" t="s">
         <v>13</v>
       </c>
@@ -1422,28 +1410,28 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.140625" style="10" customWidth="1"/>
-    <col min="2" max="2" width="32.42578125" style="10" customWidth="1"/>
+    <col min="1" max="1" width="8.5703125" style="10" customWidth="1"/>
+    <col min="2" max="2" width="55" style="10" customWidth="1"/>
     <col min="3" max="4" width="12.7109375" style="10" customWidth="1"/>
     <col min="5" max="8" width="18.28515625" style="10" customWidth="1"/>
     <col min="9" max="9" width="22.85546875" style="10" customWidth="1"/>
-    <col min="10" max="10" width="29.42578125" style="10" customWidth="1"/>
+    <col min="10" max="10" width="32" style="10" customWidth="1"/>
     <col min="11" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59"/>
-      <c r="J1" s="59"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
     </row>
     <row r="2" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
@@ -1474,58 +1462,58 @@
       <c r="J3" s="11"/>
     </row>
     <row r="4" spans="1:10" s="13" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="60" t="s">
+      <c r="A4" s="56" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="58" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="58" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="58" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="58" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="58"/>
+      <c r="G4" s="58" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="58"/>
+      <c r="I4" s="58" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4" s="60" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" s="13" customFormat="1" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="57"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="59"/>
+      <c r="D5" s="59"/>
+      <c r="E5" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="62" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="62" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="62" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" s="62" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" s="62"/>
-      <c r="G4" s="62" t="s">
-        <v>6</v>
-      </c>
-      <c r="H4" s="62"/>
-      <c r="I4" s="62" t="s">
-        <v>7</v>
-      </c>
-      <c r="J4" s="64" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" s="13" customFormat="1" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="61"/>
-      <c r="B5" s="63"/>
-      <c r="C5" s="63"/>
-      <c r="D5" s="63"/>
-      <c r="E5" s="14" t="s">
+      <c r="F5" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="14" t="s">
-        <v>25</v>
-      </c>
       <c r="G5" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="I5" s="63"/>
-      <c r="J5" s="65"/>
+      <c r="I5" s="59"/>
+      <c r="J5" s="61"/>
     </row>
     <row r="6" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="15"/>
+      <c r="B6" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="16"/>
       <c r="C6" s="16"/>
       <c r="D6" s="16"/>
       <c r="E6" s="16"/>
@@ -1536,195 +1524,195 @@
       <c r="J6" s="17"/>
     </row>
     <row r="7" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="62" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="25" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="26"/>
+      <c r="B8" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="23"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="25"/>
-      <c r="J7" s="26" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="27" t="s">
+      <c r="E8" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="28" t="s">
+      <c r="F8" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="29" t="s">
+      <c r="G8" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="30" t="s">
+      <c r="H8" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="29" t="s">
+      <c r="J8" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="29" t="s">
+    </row>
+    <row r="9" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="31"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="30"/>
+    </row>
+    <row r="10" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="26"/>
+      <c r="B10" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="G8" s="29" t="s">
+      <c r="C10" s="28">
+        <v>1</v>
+      </c>
+      <c r="D10" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="29"/>
+      <c r="F10" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="H8" s="29" t="s">
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="J10" s="30"/>
+    </row>
+    <row r="11" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="26"/>
+      <c r="B11" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="28">
+        <v>1</v>
+      </c>
+      <c r="D11" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="29"/>
+      <c r="F11" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" s="29"/>
+      <c r="H11" s="29"/>
+      <c r="I11" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="J11" s="30"/>
+    </row>
+    <row r="12" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="26"/>
+      <c r="B12" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="28">
+        <v>1</v>
+      </c>
+      <c r="D12" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="29"/>
+      <c r="F12" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="G12" s="29"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="J12" s="30"/>
+    </row>
+    <row r="13" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="26"/>
+      <c r="B13" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="28">
+        <v>1</v>
+      </c>
+      <c r="D13" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="29"/>
+      <c r="F13" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="J13" s="30"/>
+    </row>
+    <row r="14" spans="1:10" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="26"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="51" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="51"/>
+      <c r="E14" s="51"/>
+      <c r="F14" s="47" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="47"/>
+      <c r="H14" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="I8" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="J8" s="31" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="32"/>
-      <c r="B9" s="28"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="30"/>
-      <c r="H9" s="29"/>
-      <c r="I9" s="29"/>
-      <c r="J9" s="31"/>
-    </row>
-    <row r="10" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" s="28"/>
-      <c r="C10" s="29">
-        <v>1</v>
-      </c>
-      <c r="D10" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="30"/>
-      <c r="F10" s="29" t="s">
-        <v>37</v>
-      </c>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="29" t="s">
-        <v>37</v>
-      </c>
-      <c r="J10" s="31"/>
-    </row>
-    <row r="11" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="27" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11" s="28"/>
-      <c r="C11" s="29">
-        <v>1</v>
-      </c>
-      <c r="D11" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="30"/>
-      <c r="F11" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="G11" s="30"/>
-      <c r="H11" s="30"/>
-      <c r="I11" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="J11" s="31"/>
-    </row>
-    <row r="12" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" s="28"/>
-      <c r="C12" s="29">
-        <v>1</v>
-      </c>
-      <c r="D12" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" s="30"/>
-      <c r="F12" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="G12" s="30"/>
-      <c r="H12" s="30"/>
-      <c r="I12" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="J12" s="31"/>
-    </row>
-    <row r="13" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="B13" s="28"/>
-      <c r="C13" s="29">
-        <v>1</v>
-      </c>
-      <c r="D13" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="30"/>
-      <c r="F13" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="G13" s="30"/>
-      <c r="H13" s="30"/>
-      <c r="I13" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="J13" s="31"/>
-    </row>
-    <row r="14" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="27"/>
-      <c r="B14" s="28"/>
-      <c r="C14" s="57" t="s">
-        <v>44</v>
-      </c>
-      <c r="D14" s="57"/>
-      <c r="E14" s="57"/>
-      <c r="F14" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="G14" s="29"/>
-      <c r="H14" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="I14" s="29" t="s">
+      <c r="I14" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="J14" s="31"/>
+      <c r="J14" s="30"/>
     </row>
     <row r="15" spans="1:10" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="34"/>
-      <c r="B15" s="35"/>
-      <c r="C15" s="36"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="37"/>
-      <c r="H15" s="37"/>
-      <c r="I15" s="37"/>
-      <c r="J15" s="38"/>
+      <c r="A15" s="33"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="63"/>
+      <c r="D15" s="63"/>
+      <c r="E15" s="64"/>
+      <c r="F15" s="64"/>
+      <c r="G15" s="64"/>
+      <c r="H15" s="64"/>
+      <c r="I15" s="64"/>
+      <c r="J15" s="35"/>
     </row>
     <row r="16" spans="1:10" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="18"/>
       <c r="B16" s="19"/>
-      <c r="C16" s="58" t="s">
+      <c r="C16" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="58"/>
-      <c r="E16" s="58"/>
-      <c r="F16" s="58"/>
-      <c r="G16" s="58"/>
+      <c r="D16" s="54"/>
+      <c r="E16" s="54"/>
+      <c r="F16" s="54"/>
+      <c r="G16" s="54"/>
       <c r="H16" s="20" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
Update html and excel forms.
</commit_message>
<xml_diff>
--- a/Estimation.WebApi/Forms/Estimation_DetailForm.xlsx
+++ b/Estimation.WebApi/Forms/Estimation_DetailForm.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mattanapol.K\Source\Repos\EstimationServer\Estimation.WebApi\Forms\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mattanapol.K\source\repos\EstimationServer\Estimation.WebApi\Forms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FA186AB-2BFA-4A22-BA7E-D1930B48931C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9308FDF0-07BC-45B9-B1E2-20CC6F47A021}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="1">Description!$1:$5</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Summary!$4:$4</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="171027" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -165,7 +165,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -186,17 +186,29 @@
       <family val="1"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color rgb="FF000000"/>
-      <name val="AngsanaUPC"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
       <family val="1"/>
     </font>
     <font>
       <b/>
-      <sz val="14"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="AngsanaUPC"/>
+      <name val="Times New Roman"/>
       <family val="1"/>
     </font>
   </fonts>
@@ -226,7 +238,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -245,51 +257,6 @@
     </border>
     <border>
       <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-0.14996795556505021"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.14996795556505021"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-0.14996795556505021"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.14996795556505021"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="thin">
@@ -397,17 +364,47 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color theme="0" tint="-0.14996795556505021"/>
+        <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color theme="0" tint="-0.14996795556505021"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -416,7 +413,170 @@
         <color rgb="FF000000"/>
       </left>
       <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
         <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
       </right>
       <top/>
       <bottom style="thin">
@@ -426,10 +586,10 @@
     </border>
     <border>
       <left style="thin">
-        <color theme="0" tint="-0.34998626667073579"/>
+        <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color theme="0" tint="-0.34998626667073579"/>
+        <color rgb="FF000000"/>
       </right>
       <top/>
       <bottom style="thin">
@@ -439,7 +599,7 @@
     </border>
     <border>
       <left style="thin">
-        <color theme="0" tint="-0.34998626667073579"/>
+        <color rgb="FF000000"/>
       </left>
       <right style="medium">
         <color rgb="FF000000"/>
@@ -451,210 +611,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.34998626667073579"/>
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
       </top>
       <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -662,7 +629,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -673,188 +640,179 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -871,6 +829,116 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>427615</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{49AF67FC-2DED-456C-8C26-F92176F549E9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="1276350" cy="427615"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>704850</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>427615</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3946CB5C-DD05-4B16-8499-4069CD805442}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="1276350" cy="427615"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1186,197 +1254,197 @@
     <col min="9" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+    <row r="1" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
     </row>
     <row r="2" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="4" t="s">
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="8" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-    </row>
-    <row r="4" spans="1:9" s="5" customFormat="1" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="48" t="s">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+    </row>
+    <row r="4" spans="1:9" s="4" customFormat="1" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="49" t="s">
+      <c r="B4" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="49" t="s">
+      <c r="C4" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="49" t="s">
+      <c r="D4" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="49" t="s">
+      <c r="E4" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="49" t="s">
+      <c r="F4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="49" t="s">
+      <c r="G4" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="50" t="s">
+      <c r="H4" s="22" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="36"/>
-      <c r="B5" s="37" t="s">
+      <c r="A5" s="23"/>
+      <c r="B5" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="40"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="27"/>
     </row>
     <row r="6" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="32">
+      <c r="C6" s="30">
         <v>1</v>
       </c>
-      <c r="D6" s="32" t="s">
+      <c r="D6" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="28" t="s">
+      <c r="E6" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="28" t="s">
+      <c r="F6" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="28" t="s">
+      <c r="G6" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="30" t="s">
+      <c r="H6" s="32" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="31"/>
-      <c r="B7" s="27" t="s">
+      <c r="A7" s="28"/>
+      <c r="B7" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="32">
+      <c r="C7" s="30">
         <v>1</v>
       </c>
-      <c r="D7" s="32" t="s">
+      <c r="D7" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="28" t="s">
+      <c r="E7" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="28" t="s">
+      <c r="F7" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="28" t="s">
+      <c r="G7" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="30" t="s">
+      <c r="H7" s="32" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="31"/>
-      <c r="B8" s="32" t="s">
+      <c r="A8" s="28"/>
+      <c r="B8" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="32">
+      <c r="C8" s="30">
         <v>1</v>
       </c>
-      <c r="D8" s="32" t="s">
+      <c r="D8" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="28" t="s">
+      <c r="E8" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="28" t="s">
+      <c r="F8" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="28" t="s">
+      <c r="G8" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="30"/>
+      <c r="H8" s="32"/>
     </row>
     <row r="9" spans="1:9" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="31"/>
-      <c r="B9" s="28"/>
-      <c r="C9" s="51" t="s">
+      <c r="A9" s="28"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="51"/>
-      <c r="E9" s="47" t="s">
+      <c r="D9" s="33"/>
+      <c r="E9" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="47" t="s">
+      <c r="F9" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="47" t="s">
+      <c r="G9" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="H9" s="30"/>
+      <c r="H9" s="32"/>
     </row>
     <row r="10" spans="1:9" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="41"/>
-      <c r="B10" s="42"/>
-      <c r="C10" s="44"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="45"/>
-      <c r="F10" s="45"/>
-      <c r="G10" s="46"/>
-      <c r="H10" s="43"/>
+      <c r="A10" s="35"/>
+      <c r="B10" s="36"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="40"/>
     </row>
     <row r="11" spans="1:9" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="6"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="53" t="s">
+      <c r="A11" s="41"/>
+      <c r="B11" s="42"/>
+      <c r="C11" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="53"/>
-      <c r="E11" s="8" t="s">
+      <c r="D11" s="43"/>
+      <c r="E11" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F11" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="8" t="s">
+      <c r="G11" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="H11" s="9"/>
+      <c r="H11" s="45"/>
     </row>
     <row r="12" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
@@ -1397,6 +1465,7 @@
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.39370078740157483" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="71" fitToWidth="0" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1410,316 +1479,316 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" style="10" customWidth="1"/>
-    <col min="2" max="2" width="55" style="10" customWidth="1"/>
-    <col min="3" max="4" width="12.7109375" style="10" customWidth="1"/>
-    <col min="5" max="8" width="18.28515625" style="10" customWidth="1"/>
-    <col min="9" max="9" width="22.85546875" style="10" customWidth="1"/>
-    <col min="10" max="10" width="32" style="10" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="10"/>
+    <col min="1" max="1" width="8.5703125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="55" style="5" customWidth="1"/>
+    <col min="3" max="4" width="12.7109375" style="5" customWidth="1"/>
+    <col min="5" max="8" width="18.28515625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="22.85546875" style="5" customWidth="1"/>
+    <col min="10" max="10" width="32" style="5" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="55" t="s">
+    <row r="1" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="55"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
     </row>
     <row r="2" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="12" t="s">
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="8" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-    </row>
-    <row r="4" spans="1:10" s="13" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="56" t="s">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+    </row>
+    <row r="4" spans="1:10" s="6" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="58" t="s">
+      <c r="B4" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="58" t="s">
+      <c r="C4" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="58" t="s">
+      <c r="D4" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="58" t="s">
+      <c r="E4" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="58"/>
-      <c r="G4" s="58" t="s">
+      <c r="F4" s="16"/>
+      <c r="G4" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="58"/>
-      <c r="I4" s="58" t="s">
+      <c r="H4" s="16"/>
+      <c r="I4" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="60" t="s">
+      <c r="J4" s="18" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="13" customFormat="1" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="57"/>
-      <c r="B5" s="59"/>
-      <c r="C5" s="59"/>
-      <c r="D5" s="59"/>
-      <c r="E5" s="14" t="s">
+    <row r="5" spans="1:10" s="6" customFormat="1" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="15"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="H5" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="59"/>
-      <c r="J5" s="61"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="19"/>
     </row>
     <row r="6" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="15"/>
-      <c r="B6" s="16" t="s">
+      <c r="A6" s="10"/>
+      <c r="B6" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="17"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="12"/>
     </row>
     <row r="7" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="62" t="s">
+      <c r="A7" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="24"/>
-      <c r="J7" s="25" t="s">
+      <c r="C7" s="48"/>
+      <c r="D7" s="48"/>
+      <c r="E7" s="48"/>
+      <c r="F7" s="48"/>
+      <c r="G7" s="48"/>
+      <c r="H7" s="48"/>
+      <c r="I7" s="49"/>
+      <c r="J7" s="50" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="26"/>
-      <c r="B8" s="27" t="s">
+      <c r="A8" s="51"/>
+      <c r="B8" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="28" t="s">
+      <c r="C8" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="29" t="s">
+      <c r="D8" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="28" t="s">
+      <c r="E8" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="28" t="s">
+      <c r="F8" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="G8" s="28" t="s">
+      <c r="G8" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="H8" s="28" t="s">
+      <c r="H8" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="I8" s="28" t="s">
+      <c r="I8" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="J8" s="30" t="s">
+      <c r="J8" s="32" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="31"/>
-      <c r="B9" s="27"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="30"/>
+      <c r="A9" s="28"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="32"/>
     </row>
     <row r="10" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="26"/>
-      <c r="B10" s="27" t="s">
+      <c r="A10" s="51"/>
+      <c r="B10" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="28">
+      <c r="C10" s="31">
         <v>1</v>
       </c>
-      <c r="D10" s="29" t="s">
+      <c r="D10" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="29"/>
-      <c r="F10" s="28" t="s">
+      <c r="E10" s="30"/>
+      <c r="F10" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="G10" s="29"/>
-      <c r="H10" s="29"/>
-      <c r="I10" s="28" t="s">
+      <c r="G10" s="30"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="J10" s="30"/>
+      <c r="J10" s="32"/>
     </row>
     <row r="11" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="26"/>
-      <c r="B11" s="27" t="s">
+      <c r="A11" s="51"/>
+      <c r="B11" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="28">
+      <c r="C11" s="31">
         <v>1</v>
       </c>
-      <c r="D11" s="29" t="s">
+      <c r="D11" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="29"/>
-      <c r="F11" s="28" t="s">
+      <c r="E11" s="30"/>
+      <c r="F11" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="G11" s="29"/>
-      <c r="H11" s="29"/>
-      <c r="I11" s="28" t="s">
+      <c r="G11" s="30"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="J11" s="30"/>
+      <c r="J11" s="32"/>
     </row>
     <row r="12" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="26"/>
-      <c r="B12" s="27" t="s">
+      <c r="A12" s="51"/>
+      <c r="B12" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="28">
+      <c r="C12" s="31">
         <v>1</v>
       </c>
-      <c r="D12" s="29" t="s">
+      <c r="D12" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="29"/>
-      <c r="F12" s="28" t="s">
+      <c r="E12" s="30"/>
+      <c r="F12" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="G12" s="29"/>
-      <c r="H12" s="29"/>
-      <c r="I12" s="28" t="s">
+      <c r="G12" s="30"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="J12" s="30"/>
+      <c r="J12" s="32"/>
     </row>
     <row r="13" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="26"/>
-      <c r="B13" s="27" t="s">
+      <c r="A13" s="51"/>
+      <c r="B13" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="C13" s="28">
+      <c r="C13" s="31">
         <v>1</v>
       </c>
-      <c r="D13" s="29" t="s">
+      <c r="D13" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="29"/>
-      <c r="F13" s="28" t="s">
+      <c r="E13" s="30"/>
+      <c r="F13" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="G13" s="29"/>
-      <c r="H13" s="29"/>
-      <c r="I13" s="28" t="s">
+      <c r="G13" s="30"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="J13" s="30"/>
+      <c r="J13" s="32"/>
     </row>
     <row r="14" spans="1:10" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="26"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="51" t="s">
+      <c r="A14" s="51"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="D14" s="51"/>
-      <c r="E14" s="51"/>
-      <c r="F14" s="47" t="s">
+      <c r="D14" s="33"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="G14" s="47"/>
-      <c r="H14" s="47" t="s">
+      <c r="G14" s="34"/>
+      <c r="H14" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="I14" s="47" t="s">
+      <c r="I14" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="J14" s="30"/>
+      <c r="J14" s="32"/>
     </row>
     <row r="15" spans="1:10" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="33"/>
-      <c r="B15" s="34"/>
-      <c r="C15" s="63"/>
-      <c r="D15" s="63"/>
-      <c r="E15" s="64"/>
-      <c r="F15" s="64"/>
-      <c r="G15" s="64"/>
-      <c r="H15" s="64"/>
-      <c r="I15" s="64"/>
-      <c r="J15" s="35"/>
+      <c r="A15" s="52"/>
+      <c r="B15" s="53"/>
+      <c r="C15" s="54"/>
+      <c r="D15" s="54"/>
+      <c r="E15" s="55"/>
+      <c r="F15" s="55"/>
+      <c r="G15" s="55"/>
+      <c r="H15" s="55"/>
+      <c r="I15" s="55"/>
+      <c r="J15" s="56"/>
     </row>
     <row r="16" spans="1:10" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="18"/>
-      <c r="B16" s="19"/>
-      <c r="C16" s="54" t="s">
+      <c r="A16" s="57"/>
+      <c r="B16" s="58"/>
+      <c r="C16" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="54"/>
-      <c r="E16" s="54"/>
-      <c r="F16" s="54"/>
-      <c r="G16" s="54"/>
-      <c r="H16" s="20" t="s">
+      <c r="D16" s="59"/>
+      <c r="E16" s="59"/>
+      <c r="F16" s="59"/>
+      <c r="G16" s="59"/>
+      <c r="H16" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="I16" s="20" t="s">
+      <c r="I16" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="J16" s="21"/>
+      <c r="J16" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -1737,5 +1806,6 @@
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.39370078740157483" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="60" fitToWidth="0" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>